<commit_message>
fix metabolites nutrition file
</commit_message>
<xml_diff>
--- a/LGC_Motiv_analysis/nutrition/taux.xlsx
+++ b/LGC_Motiv_analysis/nutrition/taux.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhatanhdao/Documents/Projet de Bachelor travail/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhatanhdao/Documents/Projet de Bachelor rendu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DB4B10-7F53-8D4E-B04A-66242D49813F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A410C45D-17BD-F243-9B94-ECCB5B89847F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{1707A41E-2127-944B-9530-FAB8E43081B2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{1707A41E-2127-944B-9530-FAB8E43081B2}"/>
   </bookViews>
   <sheets>
     <sheet name="AFTER CONV" sheetId="2" r:id="rId1"/>
@@ -705,7 +705,7 @@
   <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2119,23 +2119,23 @@
       </c>
       <c r="B57">
         <f>'BEFORE CONV'!B57*'BEFORE CONV'!G57</f>
-        <v>0</v>
+        <v>391</v>
       </c>
       <c r="C57">
         <f>'BEFORE CONV'!C57*'BEFORE CONV'!G57</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D57">
         <f>'BEFORE CONV'!D57*'BEFORE CONV'!G57</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E57">
         <f>'BEFORE CONV'!E57*'BEFORE CONV'!G57</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F57">
         <f>'BEFORE CONV'!F57*'BEFORE CONV'!G57</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B77">
         <f>'BEFORE CONV'!B77*'BEFORE CONV'!G77</f>
-        <v>0</v>
+        <v>0.23500000000000001</v>
       </c>
       <c r="C77">
         <f>'BEFORE CONV'!C77*'BEFORE CONV'!G77</f>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="B78">
         <f>'BEFORE CONV'!B78*'BEFORE CONV'!G78</f>
-        <v>0</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="C78">
         <f>'BEFORE CONV'!C78*'BEFORE CONV'!G78</f>
@@ -2897,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166717F2-E182-F349-B994-9EFBA99CFF32}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:F48"/>
+    <sheetView topLeftCell="A53" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4255,6 +4255,9 @@
       <c r="F57">
         <v>18</v>
       </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -4726,6 +4729,10 @@
       <c r="F77">
         <v>0</v>
       </c>
+      <c r="G77">
+        <f>5*0.001</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -4745,6 +4752,10 @@
       </c>
       <c r="F78">
         <v>0</v>
+      </c>
+      <c r="G78">
+        <f>5*0.001</f>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
major update for nutrition data
</commit_message>
<xml_diff>
--- a/LGC_Motiv_analysis/nutrition/taux.xlsx
+++ b/LGC_Motiv_analysis/nutrition/taux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clairis\Desktop\GitHub\LGC_motiv\LGC_Motiv_analysis\nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902C312C-0839-400B-9721-EC73D592566C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603227E-44F8-45E2-9467-1DF516D13D8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1707A41E-2127-944B-9530-FAB8E43081B2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="347">
   <si>
     <t>Question</t>
   </si>
@@ -1164,6 +1164,9 @@
       </rPr>
       <t>]</t>
     </r>
+  </si>
+  <si>
+    <t>Energie [kcal]</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF765684-8B7E-2D4B-ABA8-2D28FB30B5F3}">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>346</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>89</v>

</xml_diff>